<commit_message>
Tune linear window size
</commit_message>
<xml_diff>
--- a/data/2019-11-01/cmpnds_tested_as_of_2019-11-01.xlsx
+++ b/data/2019-11-01/cmpnds_tested_as_of_2019-11-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/University_of_Minnesota/Wackett_Lab/github/synbio-data-analysis/data/2019-11-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0113D823-FFF1-CA4E-84B6-1ED4EC9F1FE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDFC777-0EEA-8148-826D-EC4BD613F912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36220" yWindow="6400" windowWidth="22820" windowHeight="14800" xr2:uid="{05FBBE67-27AD-554B-8C65-1DCC990B72ED}"/>
+    <workbookView xWindow="-27040" yWindow="1200" windowWidth="22820" windowHeight="14800" xr2:uid="{05FBBE67-27AD-554B-8C65-1DCC990B72ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>SMILES</t>
   </si>
@@ -84,9 +84,6 @@
     <t>O=[N+](C1=CC=C(OC(CCOC2=CC=C(Cl)C=C2)=O)C=C1)[O-]</t>
   </si>
   <si>
-    <t>O=[N+](C1=CC=C(OC(C2=CC=CC=C2)=O)C=C1)[O-]</t>
-  </si>
-  <si>
     <t>O=[N+](C1=CC=C(OC(CCCCCCCCCCC)=O)C=C1)[O-]</t>
   </si>
   <si>
@@ -94,19 +91,243 @@
   </si>
   <si>
     <t>O=[N+](C1=CC=C(OC(CCCCCCC2=CC=CC=C2)=O)C=C1)[O-]</t>
+  </si>
+  <si>
+    <t>C1=CC=C(C=C1)C(=O)OC2=CC=C(C=C2)[N+](=O)[O-]</t>
+  </si>
+  <si>
+    <t>IUPAC</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 3-(4-chlorophenoxy)propanoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl hept-6-ynoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl benzoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 7-phenylheptanoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl pivalate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl dodecanoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 2-(2-butoxyethoxy)acetate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 6-azidohexanoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 2,2-dimethylhexanoate</t>
+  </si>
+  <si>
+    <t>dimethyl</t>
+  </si>
+  <si>
+    <t>CCCCC(C)(C)C(OC1=CC=C([N+]([O-])=O)C=C1)=O</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl (3-methylbutanoyl)glycinate</t>
+  </si>
+  <si>
+    <t>glycinate</t>
+  </si>
+  <si>
+    <t>O=C(OC1=CC=C([N+]([O-])=O)C=C1)CNC(CC(C)C)=O</t>
+  </si>
+  <si>
+    <t>sulfinyl</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 2-((furan-2-ylmethyl)sulfinyl)acetate</t>
+  </si>
+  <si>
+    <t>O=C(OC1=CC=C([N+]([O-])=O)C=C1)CS(CC2=CC=CO2)=O</t>
+  </si>
+  <si>
+    <t>furan</t>
+  </si>
+  <si>
+    <t>O=C(OC1=CC=C([N+]([O-])=O)C=C1)CCC2=NN=C(C3=CC=CC=C3)O2</t>
+  </si>
+  <si>
+    <t>oxidazol</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 3-(5-phenyl-1,3,4-oxadiazol-2-yl)propanoate</t>
+  </si>
+  <si>
+    <t>cyclopent</t>
+  </si>
+  <si>
+    <t>O=C(CCC1CCCC1)CC2=CC=C([N+]([O-])=O)C=C2</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl 4-cyclopentylbutan-2-one</t>
+  </si>
+  <si>
+    <t>hexanoate</t>
+  </si>
+  <si>
+    <t>heptanoate</t>
+  </si>
+  <si>
+    <t>not_tested</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl hexanoate</t>
+  </si>
+  <si>
+    <t>4-nitrophenyl heptanoate</t>
+  </si>
+  <si>
+    <r>
+      <t>4-nitrophenyl 5-((3a</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,4</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,6a</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)-2-oxohexahydro-1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-thieno[3,4-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]imidazol-4-yl)pentanoate</t>
+    </r>
+  </si>
+  <si>
+    <t>CCCCCC(OC1=CC=C([N+]([O-])=O)C=C1)=O</t>
+  </si>
+  <si>
+    <t>CCCCCCC(OC1=CC=C([N+]([O-])=O)C=C1)=O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,8 +350,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,125 +669,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975348D5-CFA5-D94F-952C-9122A20E1B68}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>